<commit_message>
Task040: llenado de formatos de vicerrecotiría y plan de trabajo
</commit_message>
<xml_diff>
--- a/backend/app/services/documents/templates/plantilla_plan_ext.xlsx
+++ b/backend/app/services/documents/templates/plantilla_plan_ext.xlsx
@@ -1114,11 +1114,11 @@
   </sheetPr>
   <dimension ref="A1:L1012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.43"/>
@@ -15504,13 +15504,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1012"/>
+  <dimension ref="A1:L1017"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.29"/>
@@ -15999,242 +15999,242 @@
       <c r="L31" s="39"/>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="66"/>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="66"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="68"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="72"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="84"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="61"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="84"/>
+      <c r="J34" s="84"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+    </row>
+    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="61"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="84"/>
+      <c r="I35" s="84"/>
+      <c r="J35" s="84"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+    </row>
+    <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="61"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="84"/>
+      <c r="I36" s="84"/>
+      <c r="J36" s="84"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+    </row>
+    <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="66"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+    </row>
+    <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="68"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="72"/>
+    </row>
+    <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="85"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85" t="s">
+      <c r="B39" s="85"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="85"/>
-      <c r="J34" s="85"/>
-      <c r="K34" s="85"/>
-      <c r="L34" s="85"/>
-    </row>
-    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="38" t="s">
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="85"/>
+    </row>
+    <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B40" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="86" t="s">
+      <c r="C40" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
-      <c r="J35" s="87"/>
-      <c r="K35" s="87"/>
-      <c r="L35" s="87"/>
-    </row>
-    <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="30" t="s">
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="87"/>
+      <c r="I40" s="87"/>
+      <c r="J40" s="87"/>
+      <c r="K40" s="87"/>
+      <c r="L40" s="87"/>
+    </row>
+    <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="88"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="87"/>
-      <c r="I36" s="87"/>
-      <c r="J36" s="87"/>
-      <c r="K36" s="87"/>
-      <c r="L36" s="87"/>
-    </row>
-    <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="30" t="s">
+      <c r="B41" s="53"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="87"/>
+      <c r="I41" s="87"/>
+      <c r="J41" s="87"/>
+      <c r="K41" s="87"/>
+      <c r="L41" s="87"/>
+    </row>
+    <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="53"/>
-      <c r="C37" s="88"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="87"/>
-      <c r="J37" s="87"/>
-      <c r="K37" s="87"/>
-      <c r="L37" s="87"/>
-    </row>
-    <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30" t="s">
+      <c r="B42" s="53"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="87"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="87"/>
+      <c r="L42" s="87"/>
+    </row>
+    <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="88"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="87"/>
-      <c r="I38" s="87"/>
-      <c r="J38" s="87"/>
-      <c r="K38" s="87"/>
-      <c r="L38" s="87"/>
-    </row>
-    <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="30" t="s">
+      <c r="B43" s="53"/>
+      <c r="C43" s="88"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="87"/>
+      <c r="F43" s="87"/>
+      <c r="G43" s="87"/>
+      <c r="H43" s="87"/>
+      <c r="I43" s="87"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="87"/>
+      <c r="L43" s="87"/>
+    </row>
+    <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="53"/>
-      <c r="C39" s="88"/>
-      <c r="D39" s="87"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87"/>
-      <c r="H39" s="87"/>
-      <c r="I39" s="87"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
-      <c r="L39" s="87"/>
-    </row>
-    <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="30" t="s">
+      <c r="B44" s="53"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="87"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="87"/>
+    </row>
+    <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="53"/>
-      <c r="C40" s="88"/>
-      <c r="D40" s="89" t="s">
+      <c r="B45" s="53"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="89"/>
-      <c r="F40" s="89" t="s">
+      <c r="E45" s="89"/>
+      <c r="F45" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="G40" s="89"/>
-      <c r="H40" s="89"/>
-      <c r="I40" s="89" t="s">
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="J40" s="89"/>
-      <c r="K40" s="89"/>
-      <c r="L40" s="89"/>
-    </row>
-    <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="30" t="s">
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
+    </row>
+    <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="89"/>
-      <c r="I41" s="89"/>
-      <c r="J41" s="89"/>
-      <c r="K41" s="89"/>
-      <c r="L41" s="89"/>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="91"/>
-      <c r="B42" s="91"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="91"/>
-      <c r="H42" s="91"/>
-      <c r="I42" s="91"/>
-      <c r="J42" s="91"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="91"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="91"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="91"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="91"/>
-      <c r="B44" s="91"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="91"/>
-      <c r="G44" s="91"/>
-      <c r="H44" s="91"/>
-      <c r="I44" s="91"/>
-      <c r="J44" s="91"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="91"/>
-      <c r="B45" s="91"/>
-      <c r="C45" s="92"/>
-      <c r="D45" s="91"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="91"/>
-      <c r="H45" s="91"/>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="91"/>
-      <c r="B46" s="91"/>
-      <c r="C46" s="92"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="91"/>
-      <c r="G46" s="91"/>
-      <c r="H46" s="91"/>
-      <c r="I46" s="91"/>
-      <c r="J46" s="91"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
+      <c r="I46" s="89"/>
+      <c r="J46" s="89"/>
+      <c r="K46" s="89"/>
+      <c r="L46" s="89"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="91"/>
@@ -29760,8 +29760,78 @@
       <c r="K1012" s="13"/>
       <c r="L1012" s="13"/>
     </row>
+    <row r="1013" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1013" s="91"/>
+      <c r="B1013" s="91"/>
+      <c r="C1013" s="92"/>
+      <c r="D1013" s="91"/>
+      <c r="E1013" s="13"/>
+      <c r="F1013" s="91"/>
+      <c r="G1013" s="91"/>
+      <c r="H1013" s="91"/>
+      <c r="I1013" s="91"/>
+      <c r="J1013" s="91"/>
+      <c r="K1013" s="13"/>
+      <c r="L1013" s="13"/>
+    </row>
+    <row r="1014" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1014" s="91"/>
+      <c r="B1014" s="91"/>
+      <c r="C1014" s="92"/>
+      <c r="D1014" s="91"/>
+      <c r="E1014" s="13"/>
+      <c r="F1014" s="91"/>
+      <c r="G1014" s="91"/>
+      <c r="H1014" s="91"/>
+      <c r="I1014" s="91"/>
+      <c r="J1014" s="91"/>
+      <c r="K1014" s="13"/>
+      <c r="L1014" s="13"/>
+    </row>
+    <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1015" s="91"/>
+      <c r="B1015" s="91"/>
+      <c r="C1015" s="92"/>
+      <c r="D1015" s="91"/>
+      <c r="E1015" s="13"/>
+      <c r="F1015" s="91"/>
+      <c r="G1015" s="91"/>
+      <c r="H1015" s="91"/>
+      <c r="I1015" s="91"/>
+      <c r="J1015" s="91"/>
+      <c r="K1015" s="13"/>
+      <c r="L1015" s="13"/>
+    </row>
+    <row r="1016" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1016" s="91"/>
+      <c r="B1016" s="91"/>
+      <c r="C1016" s="92"/>
+      <c r="D1016" s="91"/>
+      <c r="E1016" s="13"/>
+      <c r="F1016" s="91"/>
+      <c r="G1016" s="91"/>
+      <c r="H1016" s="91"/>
+      <c r="I1016" s="91"/>
+      <c r="J1016" s="91"/>
+      <c r="K1016" s="13"/>
+      <c r="L1016" s="13"/>
+    </row>
+    <row r="1017" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1017" s="91"/>
+      <c r="B1017" s="91"/>
+      <c r="C1017" s="92"/>
+      <c r="D1017" s="91"/>
+      <c r="E1017" s="13"/>
+      <c r="F1017" s="91"/>
+      <c r="G1017" s="91"/>
+      <c r="H1017" s="91"/>
+      <c r="I1017" s="91"/>
+      <c r="J1017" s="91"/>
+      <c r="K1017" s="13"/>
+      <c r="L1017" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="68">
+  <mergeCells count="83">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:L3"/>
@@ -29823,13 +29893,28 @@
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="H31:J31"/>
     <mergeCell ref="K31:L31"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:L34"/>
-    <mergeCell ref="D35:L39"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="F40:H41"/>
-    <mergeCell ref="I40:L41"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:L39"/>
+    <mergeCell ref="D40:L44"/>
+    <mergeCell ref="D45:E46"/>
+    <mergeCell ref="F45:H46"/>
+    <mergeCell ref="I45:L46"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>